<commit_message>
Plot Meziadin total return by year and sibling reg point forecast with 25/75th percentile error bars
</commit_message>
<xml_diff>
--- a/data/mez_predictions.xlsx
+++ b/data/mez_predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/nass-data-summaries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D359A88-4D53-4140-AAAA-89D3C547AC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B4F68-15CA-D54F-B350-139CEF302A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
+    <workbookView xWindow="1200" yWindow="3360" windowWidth="27600" windowHeight="16940" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>predicted return</t>
   </si>
   <si>
     <t>runyear</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p75</t>
   </si>
 </sst>
 </file>
@@ -85,12 +91,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,11 +118,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}" name="Table1" displayName="Table1" ref="A1:B15" totalsRowShown="0">
-  <autoFilter ref="A1:B15" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -433,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977606BB-721A-1F49-A8B4-EAA00C781FFB}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,124 +458,214 @@
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2012</v>
       </c>
       <c r="B2" s="1">
         <v>478892</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="2">
+        <v>287613</v>
+      </c>
+      <c r="D2" s="2">
+        <v>651471</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2013</v>
       </c>
       <c r="B3" s="1">
         <v>373898</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2">
+        <v>236161</v>
+      </c>
+      <c r="D3" s="2">
+        <v>605663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2014</v>
       </c>
       <c r="B4" s="1">
         <v>463016</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="2">
+        <v>327560</v>
+      </c>
+      <c r="D4" s="2">
+        <v>633701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2015</v>
       </c>
       <c r="B5" s="1">
         <v>422914</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="2">
+        <v>278110</v>
+      </c>
+      <c r="D5" s="2">
+        <v>597477</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2016</v>
       </c>
       <c r="B6" s="1">
         <v>413089</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="2">
+        <v>285478</v>
+      </c>
+      <c r="D6" s="2">
+        <v>567755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2017</v>
       </c>
       <c r="B7" s="1">
         <v>144864</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="2">
+        <v>112488</v>
+      </c>
+      <c r="D7" s="2">
+        <v>309076</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2018</v>
       </c>
       <c r="B8" s="1">
         <v>200293</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="2">
+        <v>137562</v>
+      </c>
+      <c r="D8" s="2">
+        <v>339044</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2019</v>
       </c>
       <c r="B9" s="1">
         <v>208034</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="2">
+        <v>133096</v>
+      </c>
+      <c r="D9" s="2">
+        <v>339139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2020</v>
       </c>
       <c r="B10" s="1">
         <v>209793</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="2">
+        <v>133189</v>
+      </c>
+      <c r="D10" s="2">
+        <v>331119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2021</v>
       </c>
       <c r="B11" s="1">
         <v>148960</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="2">
+        <v>119280</v>
+      </c>
+      <c r="D11" s="2">
+        <v>309427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2022</v>
       </c>
       <c r="B12" s="1">
         <v>953767</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="2">
+        <v>775247</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1107526</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2023</v>
       </c>
       <c r="B13" s="1">
         <v>549673</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="2">
+        <v>407566</v>
+      </c>
+      <c r="D13" s="2">
+        <v>703180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2024</v>
       </c>
       <c r="B14" s="1">
         <v>627887</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="2">
+        <v>475099</v>
+      </c>
+      <c r="D14" s="2">
+        <v>774011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2025</v>
       </c>
       <c r="B15" s="1">
         <v>854359</v>
+      </c>
+      <c r="C15" s="2">
+        <v>711287</v>
+      </c>
+      <c r="D15" s="2">
+        <v>993255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data and code to create actual return vs predicted plot using NAIVE model to compare with sibling reg
</commit_message>
<xml_diff>
--- a/data/mez_predictions.xlsx
+++ b/data/mez_predictions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/nass-data-summaries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15B4F68-15CA-D54F-B350-139CEF302A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CA85F2-595B-1846-AA32-4FA76585D1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="3360" windowWidth="27600" windowHeight="16940" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" activeTab="1" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sibregsimple" sheetId="1" r:id="rId1"/>
+    <sheet name="naive" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>predicted return</t>
   </si>
@@ -91,7 +92,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -121,10 +134,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
   <autoFilter ref="A1:D15" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}" name="Table13" displayName="Table13" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C2FB065E-FF87-6C4C-BB4C-8837F14738AA}" name="runyear" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{04D1F83E-14EA-BC47-BD00-2E3527FF9AF1}" name="predicted return" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{DB26FEF8-8B80-284B-822A-7F2412FA4869}" name="p25" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EE2E5417-33B6-7C4D-89CB-56D82D53DDAF}" name="p75" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -449,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977606BB-721A-1F49-A8B4-EAA00C781FFB}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -674,4 +700,232 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4438618E-78F8-7E4A-A0D0-3FE3B2BDC728}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B2" s="1">
+        <v>342174</v>
+      </c>
+      <c r="C2" s="2">
+        <v>287001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>392441</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B3" s="1">
+        <v>315515</v>
+      </c>
+      <c r="C3" s="2">
+        <v>293819</v>
+      </c>
+      <c r="D3" s="2">
+        <v>342174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="1">
+        <v>351087</v>
+      </c>
+      <c r="C4" s="2">
+        <v>316834</v>
+      </c>
+      <c r="D4" s="2">
+        <v>381393</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="1">
+        <v>339117</v>
+      </c>
+      <c r="C5" s="2">
+        <v>298048</v>
+      </c>
+      <c r="D5" s="2">
+        <v>380526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="1">
+        <v>372239</v>
+      </c>
+      <c r="C6" s="2">
+        <v>324549</v>
+      </c>
+      <c r="D6" s="2">
+        <v>415229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="1">
+        <v>297877</v>
+      </c>
+      <c r="C7" s="2">
+        <v>234712</v>
+      </c>
+      <c r="D7" s="2">
+        <v>369710</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1">
+        <v>263094</v>
+      </c>
+      <c r="C8" s="2">
+        <v>185352</v>
+      </c>
+      <c r="D8" s="2">
+        <v>324013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B9" s="1">
+        <v>167357</v>
+      </c>
+      <c r="C9" s="2">
+        <v>141577</v>
+      </c>
+      <c r="D9" s="2">
+        <v>187773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="1">
+        <v>153755</v>
+      </c>
+      <c r="C10" s="2">
+        <v>133983</v>
+      </c>
+      <c r="D10" s="2">
+        <v>172805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B11" s="1">
+        <v>148960</v>
+      </c>
+      <c r="C11" s="2">
+        <v>134802</v>
+      </c>
+      <c r="D11" s="2">
+        <v>164863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="1">
+        <v>233795</v>
+      </c>
+      <c r="C12" s="2">
+        <v>171847</v>
+      </c>
+      <c r="D12" s="2">
+        <v>297664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B13" s="1">
+        <v>348223</v>
+      </c>
+      <c r="C13" s="2">
+        <v>267359</v>
+      </c>
+      <c r="D13" s="2">
+        <v>427068</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B14" s="1">
+        <v>478498</v>
+      </c>
+      <c r="C14" s="2">
+        <v>426099</v>
+      </c>
+      <c r="D14" s="2">
+        <v>523874</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1">
+        <v>593257</v>
+      </c>
+      <c r="C15" s="2">
+        <v>534884</v>
+      </c>
+      <c r="D15" s="2">
+        <v>654729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update resource doc and Meziadin forecast dataset for 1/27/25
</commit_message>
<xml_diff>
--- a/data/mez_predictions.xlsx
+++ b/data/mez_predictions.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/nass-data-summaries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CA85F2-595B-1846-AA32-4FA76585D1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575F525-905D-3D4A-8CE9-F5DF0B2D1A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" activeTab="1" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" activeTab="2" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
   </bookViews>
   <sheets>
     <sheet name="sibregsimple" sheetId="1" r:id="rId1"/>
     <sheet name="naive" sheetId="2" r:id="rId2"/>
+    <sheet name="nass_sibreg" sheetId="3" r:id="rId3"/>
+    <sheet name="nass_naive" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>predicted return</t>
   </si>
@@ -92,7 +94,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -134,10 +160,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
   <autoFilter ref="A1:D15" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -147,10 +173,36 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}" name="Table13" displayName="Table13" ref="A1:D15" totalsRowShown="0">
   <autoFilter ref="A1:D15" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2FB065E-FF87-6C4C-BB4C-8837F14738AA}" name="runyear" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{04D1F83E-14EA-BC47-BD00-2E3527FF9AF1}" name="predicted return" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{DB26FEF8-8B80-284B-822A-7F2412FA4869}" name="p25" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{EE2E5417-33B6-7C4D-89CB-56D82D53DDAF}" name="p75" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C2FB065E-FF87-6C4C-BB4C-8837F14738AA}" name="runyear" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{04D1F83E-14EA-BC47-BD00-2E3527FF9AF1}" name="predicted return" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{DB26FEF8-8B80-284B-822A-7F2412FA4869}" name="p25" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{EE2E5417-33B6-7C4D-89CB-56D82D53DDAF}" name="p75" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{007EED31-B317-F943-A917-8338B5A55C71}" name="Table14" displayName="Table14" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{007EED31-B317-F943-A917-8338B5A55C71}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0894F52A-FA9D-204C-BA90-99B20B80543F}" name="runyear" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{3BA75908-7281-B546-B7E5-912884914548}" name="predicted return" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9C6FF38D-1C2E-374C-A49F-705F356AA785}" name="p25" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A896D351-2E17-2248-B84B-980FF0208916}" name="p75" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14CA2F93-DF60-5D46-90F4-C072BB766D93}" name="Table145" displayName="Table145" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{14CA2F93-DF60-5D46-90F4-C072BB766D93}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{70BA872D-BDA9-9D41-8900-9A6D53B0C107}" name="runyear" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{635D51DB-48A3-DC4F-A672-1A45BFCCFAE6}" name="predicted return" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F6F010F7-53DB-954E-8369-5004285BCC32}" name="p25" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{37D87CF0-A8C3-8742-A239-DBBE1249320D}" name="p75" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -706,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4438618E-78F8-7E4A-A0D0-3FE3B2BDC728}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -928,4 +980,292 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C57DF5-B1A6-CE4B-90A9-F77BBB51256D}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C01C63D-6193-754F-B59F-C6ED6FF1C8E0}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2024</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
meziadin forecasting - save sibling regression predictions using new age-class dataset and create new actual vs predicted plot
</commit_message>
<xml_diff>
--- a/data/mez_predictions.xlsx
+++ b/data/mez_predictions.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/nass-data-summaries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9575F525-905D-3D4A-8CE9-F5DF0B2D1A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1F7EF8-456E-EB4B-9CED-226ED74A6F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" activeTab="2" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="27600" windowHeight="16940" activeTab="1" xr2:uid="{A1394B72-8617-6344-9E48-19C7886783D2}"/>
   </bookViews>
   <sheets>
     <sheet name="sibregsimple" sheetId="1" r:id="rId1"/>
     <sheet name="naive" sheetId="2" r:id="rId2"/>
-    <sheet name="nass_sibreg" sheetId="3" r:id="rId3"/>
-    <sheet name="nass_naive" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>predicted return</t>
   </si>
@@ -94,31 +92,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -160,10 +134,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
   <autoFilter ref="A1:D15" xr:uid="{3A067DBE-E900-1D48-ABE4-A911F9DA0D16}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{17605C41-3082-4848-9910-156312EDB5DF}" name="runyear" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{80BDA8B2-ED8E-1D4A-AA02-F2A578758529}" name="predicted return" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{76E422DB-C2FE-D44B-A71F-4D9E91F51139}" name="p25" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{21BD0750-C404-FE46-AF03-0E0B9336E3B7}" name="p75" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -173,36 +147,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}" name="Table13" displayName="Table13" ref="A1:D15" totalsRowShown="0">
   <autoFilter ref="A1:D15" xr:uid="{7E866731-091C-F848-BEF9-B0D081C391A3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C2FB065E-FF87-6C4C-BB4C-8837F14738AA}" name="runyear" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{04D1F83E-14EA-BC47-BD00-2E3527FF9AF1}" name="predicted return" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{DB26FEF8-8B80-284B-822A-7F2412FA4869}" name="p25" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{EE2E5417-33B6-7C4D-89CB-56D82D53DDAF}" name="p75" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{007EED31-B317-F943-A917-8338B5A55C71}" name="Table14" displayName="Table14" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15" xr:uid="{007EED31-B317-F943-A917-8338B5A55C71}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0894F52A-FA9D-204C-BA90-99B20B80543F}" name="runyear" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3BA75908-7281-B546-B7E5-912884914548}" name="predicted return" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9C6FF38D-1C2E-374C-A49F-705F356AA785}" name="p25" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{A896D351-2E17-2248-B84B-980FF0208916}" name="p75" dataDxfId="4"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14CA2F93-DF60-5D46-90F4-C072BB766D93}" name="Table145" displayName="Table145" ref="A1:D15" totalsRowShown="0">
-  <autoFilter ref="A1:D15" xr:uid="{14CA2F93-DF60-5D46-90F4-C072BB766D93}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{70BA872D-BDA9-9D41-8900-9A6D53B0C107}" name="runyear" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{635D51DB-48A3-DC4F-A672-1A45BFCCFAE6}" name="predicted return" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F6F010F7-53DB-954E-8369-5004285BCC32}" name="p25" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{37D87CF0-A8C3-8742-A239-DBBE1249320D}" name="p75" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C2FB065E-FF87-6C4C-BB4C-8837F14738AA}" name="runyear" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{04D1F83E-14EA-BC47-BD00-2E3527FF9AF1}" name="predicted return" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{DB26FEF8-8B80-284B-822A-7F2412FA4869}" name="p25" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{EE2E5417-33B6-7C4D-89CB-56D82D53DDAF}" name="p75" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -528,7 +476,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D15"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4438618E-78F8-7E4A-A0D0-3FE3B2BDC728}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -980,292 +928,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95C57DF5-B1A6-CE4B-90A9-F77BBB51256D}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2013</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>2023</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>2024</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>2025</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C01C63D-6193-754F-B59F-C6ED6FF1C8E0}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2013</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>2020</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
-        <v>2021</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>2022</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>2023</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>2024</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>2025</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>